<commit_message>
docs edits during narraiton
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1b_CO2_Fluid_Inclusions/SO2_Peak_fits.xlsx
+++ b/docs/Examples/Example1b_CO2_Fluid_Inclusions/SO2_Peak_fits.xlsx
@@ -470,7 +470,7 @@
         <v>1150.799076805806</v>
       </c>
       <c r="C2" t="n">
-        <v>547.5551415582706</v>
+        <v>556.8820601375211</v>
       </c>
       <c r="D2" t="n">
         <v>401.4956768160507</v>
@@ -491,7 +491,7 @@
         <v>1151.683997496496</v>
       </c>
       <c r="C3" t="n">
-        <v>41.78971752359785</v>
+        <v>45.47286828470842</v>
       </c>
       <c r="D3" t="n">
         <v>25.9282118822</v>
@@ -512,7 +512,7 @@
         <v>1151.182542438439</v>
       </c>
       <c r="C4" t="n">
-        <v>176.5086366792257</v>
+        <v>180.0007210602771</v>
       </c>
       <c r="D4" t="n">
         <v>121.9862880887559</v>
@@ -533,7 +533,7 @@
         <v>1150.917066231231</v>
       </c>
       <c r="C5" t="n">
-        <v>69.57609552145854</v>
+        <v>70.08344443838996</v>
       </c>
       <c r="D5" t="n">
         <v>49.68469369621323</v>
@@ -554,7 +554,7 @@
         <v>1150.769579449449</v>
       </c>
       <c r="C6" t="n">
-        <v>1171.900770000038</v>
+        <v>1193.886885480184</v>
       </c>
       <c r="D6" t="n">
         <v>847.6919894156773</v>
@@ -575,7 +575,7 @@
         <v>1150.828574162162</v>
       </c>
       <c r="C7" t="n">
-        <v>330.0877917390737</v>
+        <v>336.8006864955747</v>
       </c>
       <c r="D7" t="n">
         <v>238.2441265229412</v>
@@ -596,7 +596,7 @@
         <v>1150.769579449449</v>
       </c>
       <c r="C8" t="n">
-        <v>308.4355593728184</v>
+        <v>361.1135807444104</v>
       </c>
       <c r="D8" t="n">
         <v>220.9849404097855</v>
@@ -617,7 +617,7 @@
         <v>1151.0055583003</v>
       </c>
       <c r="C9" t="n">
-        <v>88.15764607835709</v>
+        <v>88.45279340605903</v>
       </c>
       <c r="D9" t="n">
         <v>62.87890665466512</v>

</xml_diff>